<commit_message>
Se crean metodos para agregar/actualizar y ver transportes
</commit_message>
<xml_diff>
--- a/Docs/Campos_catálogos.xlsx
+++ b/Docs/Campos_catálogos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mercader-my.sharepoint.com/personal/jaramos_almer_com_mx/Documents/Escritorio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abernal\Desktop\GESCIT\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="14_{CF6C7B17-B595-4421-8CA4-24ADB8110040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F241229A-5867-4074-B2CC-B3977B1881D7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA150CB-CAD9-443E-8F48-481C99967810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9B21D353-9024-47B8-8312-A4D4CED87ECA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9B21D353-9024-47B8-8312-A4D4CED87ECA}"/>
   </bookViews>
   <sheets>
     <sheet name="Campos" sheetId="2" r:id="rId1"/>
@@ -541,31 +541,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B878AEF2-BD0D-4550-AE42-E9368F7619D8}">
   <dimension ref="B2:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L18" sqref="L17:L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="20.6640625" customWidth="1"/>
-    <col min="5" max="5" width="21.77734375" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
-    <col min="7" max="7" width="24.6640625" customWidth="1"/>
-    <col min="8" max="8" width="28.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" customWidth="1"/>
+    <col min="8" max="8" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -585,37 +585,37 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>31</v>
       </c>
@@ -626,37 +626,37 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>9</v>
       </c>
@@ -679,7 +679,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>16</v>
       </c>
@@ -702,7 +702,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>11</v>
       </c>
@@ -725,82 +725,82 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>35</v>
       </c>

</xml_diff>